<commit_message>
added Purchase Foreign Currency testcase
</commit_message>
<xml_diff>
--- a/target/test-classes/excel/TC001VerifyLoginData.xlsx
+++ b/target/test-classes/excel/TC001VerifyLoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\eclipse-workspace\E2EzeroBankingProjectFinal\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E68A21C-C8AB-4AC5-B349-88D77C94F759}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6927279D-E670-40BC-B622-19122335BCF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5205" yWindow="1320" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>user</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>username</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,6 +389,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>